<commit_message>
Finished Legionella positivity trend graph by facility area by source, cleaned up all trend graphs with better colors, fontstyle and font sizing
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanjays/Desktop/Programming/Nalco/coc_proj/coc_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32246BEC-241B-A443-A41E-4EACDC6ADDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191FECA-B420-7746-BCFF-F8ACC37BCA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -768,10 +768,10 @@
         <v>1.2</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N6">
         <v>1238</v>
@@ -850,10 +850,10 @@
         <v>0.4</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N8">
         <v>1240</v>
@@ -891,10 +891,10 @@
         <v>0.3</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N9">
         <v>1241</v>
@@ -1090,10 +1090,10 @@
         <v>0.04</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N14">
         <v>1234</v>
@@ -1131,7 +1131,7 @@
         <v>1.2</v>
       </c>
       <c r="L15">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="M15" t="s">
         <v>36</v>
@@ -1172,10 +1172,10 @@
         <v>0.8</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N16">
         <v>1236</v>
@@ -1295,7 +1295,7 @@
         <v>0.2</v>
       </c>
       <c r="L19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M19" t="s">
         <v>36</v>
@@ -1377,10 +1377,10 @@
         <v>0.3</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N21">
         <v>1241</v>
@@ -1459,7 +1459,7 @@
         <v>0.6</v>
       </c>
       <c r="L23">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="M23" t="s">
         <v>36</v>
@@ -1535,12 +1535,984 @@
         <v>18</v>
       </c>
       <c r="L25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M25" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26">
+        <v>78</v>
+      </c>
+      <c r="J26">
+        <v>0.04</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27">
+        <v>79</v>
+      </c>
+      <c r="J27">
+        <v>1.2</v>
+      </c>
+      <c r="L27">
+        <v>60</v>
+      </c>
+      <c r="M27" t="s">
         <v>36</v>
       </c>
-      <c r="N25">
+      <c r="N27">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28">
+        <v>72</v>
+      </c>
+      <c r="K28">
+        <v>0.8</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29">
+        <v>69</v>
+      </c>
+      <c r="K29">
+        <v>1.4</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>35</v>
+      </c>
+      <c r="N29">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30">
+        <v>254</v>
+      </c>
+      <c r="H30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30">
+        <v>70</v>
+      </c>
+      <c r="K30">
+        <v>1.2</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31">
+        <v>254</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31">
+        <v>114</v>
+      </c>
+      <c r="K31">
+        <v>0.2</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32">
+        <v>259</v>
+      </c>
+      <c r="H32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32">
+        <v>116</v>
+      </c>
+      <c r="K32">
+        <v>0.4</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33">
+        <v>118</v>
+      </c>
+      <c r="K33">
+        <v>0.3</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N33">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34">
+        <v>108</v>
+      </c>
+      <c r="K34">
+        <v>0.08</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35">
+        <v>117</v>
+      </c>
+      <c r="K35">
+        <v>0.6</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35" t="s">
+        <v>35</v>
+      </c>
+      <c r="N35">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36">
+        <v>116</v>
+      </c>
+      <c r="K36">
+        <v>0.3</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>35</v>
+      </c>
+      <c r="N36">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>44461</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37" t="s">
+        <v>35</v>
+      </c>
+      <c r="N37">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38">
+        <v>78</v>
+      </c>
+      <c r="J38">
+        <v>0.04</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38" t="s">
+        <v>35</v>
+      </c>
+      <c r="N38">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39">
+        <v>79</v>
+      </c>
+      <c r="J39">
+        <v>1.2</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39" t="s">
+        <v>35</v>
+      </c>
+      <c r="N39">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40">
+        <v>72</v>
+      </c>
+      <c r="K40">
+        <v>0.8</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>35</v>
+      </c>
+      <c r="N40">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41">
+        <v>69</v>
+      </c>
+      <c r="K41">
+        <v>1.4</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>35</v>
+      </c>
+      <c r="N41">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42">
+        <v>254</v>
+      </c>
+      <c r="H42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42">
+        <v>70</v>
+      </c>
+      <c r="K42">
+        <v>1.2</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42" t="s">
+        <v>35</v>
+      </c>
+      <c r="N42">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43">
+        <v>254</v>
+      </c>
+      <c r="H43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43">
+        <v>114</v>
+      </c>
+      <c r="K43">
+        <v>0.2</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43" t="s">
+        <v>35</v>
+      </c>
+      <c r="N43">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44">
+        <v>259</v>
+      </c>
+      <c r="H44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44">
+        <v>116</v>
+      </c>
+      <c r="K44">
+        <v>0.4</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44" t="s">
+        <v>35</v>
+      </c>
+      <c r="N44">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45">
+        <v>118</v>
+      </c>
+      <c r="K45">
+        <v>0.3</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N45">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46">
+        <v>108</v>
+      </c>
+      <c r="K46">
+        <v>0.08</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46" t="s">
+        <v>35</v>
+      </c>
+      <c r="N46">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47">
+        <v>117</v>
+      </c>
+      <c r="K47">
+        <v>0.6</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47" t="s">
+        <v>35</v>
+      </c>
+      <c r="N47">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48">
+        <v>116</v>
+      </c>
+      <c r="K48">
+        <v>0.3</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48" t="s">
+        <v>35</v>
+      </c>
+      <c r="N48">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>44554</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" t="s">
+        <v>18</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
+        <v>35</v>
+      </c>
+      <c r="N49">
         <v>1245</v>
       </c>
     </row>

</xml_diff>